<commit_message>
pulls in battle redd data instead of standard and modifies according to comments from review meeting 3/21. re-writes clean redd csv
</commit_message>
<xml_diff>
--- a/data-raw/metadata/battle_redd_metadata.xlsx
+++ b/data-raw/metadata/battle_redd_metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/code/jpe-battle-adult-edi/data-raw/metadata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/code/SRJPE/EDI/jpe-battle-adult-edi/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C0CCF3C-3B5D-9746-8737-097CB4836BD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27B69B56-A4BF-8843-9EDB-7205F30DFB3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="68640" yWindow="-9480" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="66">
   <si>
     <t xml:space="preserve">attribute_name </t>
   </si>
@@ -127,24 +127,6 @@
     <t>reach</t>
   </si>
   <si>
-    <t>Survey reach where redd was located. Levels = c("R2", "R3", "R7", "R1", "R4", "R5", "R6", "R1B", "R12")</t>
-  </si>
-  <si>
-    <t xml:space="preserve">	Date on which redd data was collected</t>
-  </si>
-  <si>
-    <t>river_mile</t>
-  </si>
-  <si>
-    <t>River mile where redd was located</t>
-  </si>
-  <si>
-    <t>mile</t>
-  </si>
-  <si>
-    <t>fish_guarding</t>
-  </si>
-  <si>
     <t>redd_measured</t>
   </si>
   <si>
@@ -157,13 +139,7 @@
     <t>age</t>
   </si>
   <si>
-    <t>age_index</t>
-  </si>
-  <si>
     <t>run</t>
-  </si>
-  <si>
-    <t>Run of the fish on the redd. Levels = "not recorded"</t>
   </si>
   <si>
     <t>nominal</t>
@@ -176,9 +152,6 @@
   </si>
   <si>
     <t>pre_redd_substrate_class</t>
-  </si>
-  <si>
-    <t>Whether or not a fish was observed guarding the redd. Levels = c("NA", "TRUE", "FALSE")</t>
   </si>
   <si>
     <t>Whether or not the redd was measured at time of observation.</t>
@@ -196,24 +169,63 @@
     <t>year</t>
   </si>
   <si>
-    <t>The number of times a unique redd has been surveyed. If 0, the redd was not surveyed. Levels = c(0, 1, 2, 3, 4, 5)</t>
+    <t>redd_count</t>
   </si>
   <si>
-    <t>Size class determined by millimeter size of substrate. Levels = c(NA, "very coarse sand", "very fine gravel", "coarse sand", 
+    <t>number of redds</t>
+  </si>
+  <si>
+    <t>redd_id</t>
+  </si>
+  <si>
+    <t>Survey reach where redd was located. Levels =c("R2", "R3", "R7", "R1", "R4", "R5", "R6", "R1B")</t>
+  </si>
+  <si>
+    <t>fish_on_redd</t>
+  </si>
+  <si>
+    <t>Whether or not a fish was observed on the redd being sampled. Levels = c("NA", "TRUE", "FALSE")</t>
+  </si>
+  <si>
+    <t>Run of the fish on the redd. Levels = c("spring", NA)</t>
+  </si>
+  <si>
+    <t>Number of redds sampled.</t>
+  </si>
+  <si>
+    <t>pre_redd_depth</t>
+  </si>
+  <si>
+    <t>redd_pit_depth</t>
+  </si>
+  <si>
+    <t>redd_tail_depth</t>
+  </si>
+  <si>
+    <t>Size class determined by millimeter size of substrate, and standardized using the Wentworth scale (see Methods). Levels = c(NA, "very coarse sand", "very fine gravel", "coarse sand", 
 "medium gravel", "fine gravel", "fine sand")</t>
   </si>
   <si>
-    <t>Size class determined by millimeter size of substrate. Levels = c(NA, "very fine gravel", "very coarse sand", "coarse sand", 
+    <t>Size class determined by millimeter size of substrate, and standardized using the Wentworth scale (see Methods). Levels = c(NA, "very fine gravel", "very coarse sand", "coarse sand", 
 "fine gravel")</t>
   </si>
   <si>
-    <t>redd_count</t>
+    <t>Pre-redd depth in inches.</t>
   </si>
   <si>
-    <t>Number of redds observed</t>
+    <t>Pit depth in inches.</t>
   </si>
   <si>
-    <t>number of redds</t>
+    <t>Tailspill depth in inches.</t>
+  </si>
+  <si>
+    <t>inch</t>
+  </si>
+  <si>
+    <t>Unique redd ID assigned to the redd being sampled. One redd may have been observed multiple times, resulting in multiple rows for one redd ID.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Date on which redd data was collected.</t>
   </si>
 </sst>
 </file>
@@ -547,11 +559,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1005"/>
+  <dimension ref="A1:Z1006"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="147" zoomScaleNormal="147" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="147" zoomScaleNormal="147" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H13" sqref="H13"/>
+      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -631,7 +643,7 @@
         <v>21</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>34</v>
+        <v>65</v>
       </c>
       <c r="C2" s="13" t="s">
         <v>17</v>
@@ -672,20 +684,14 @@
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>33</v>
+        <v>64</v>
       </c>
-      <c r="C3" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="E3" s="13" t="s">
-        <v>14</v>
-      </c>
+      <c r="C3" s="13"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="13"/>
       <c r="F3" s="15"/>
       <c r="G3" s="15"/>
       <c r="H3" s="15"/>
@@ -710,38 +716,28 @@
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>26</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
-      <c r="F4" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="H4" s="15" t="s">
-        <v>28</v>
-      </c>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
       <c r="I4" s="14"/>
       <c r="J4" s="15"/>
       <c r="K4" s="14"/>
-      <c r="L4" s="15">
-        <v>0</v>
-      </c>
-      <c r="M4" s="15">
-        <v>17</v>
-      </c>
+      <c r="L4" s="16"/>
+      <c r="M4" s="16"/>
       <c r="N4" s="7"/>
       <c r="O4" s="7"/>
       <c r="P4" s="7"/>
@@ -758,10 +754,10 @@
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C5" s="13" t="s">
         <v>13</v>
@@ -796,28 +792,38 @@
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D6" s="14" t="s">
         <v>26</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
+      <c r="F6" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="H6" s="15" t="s">
+        <v>29</v>
+      </c>
       <c r="I6" s="14"/>
       <c r="J6" s="15"/>
       <c r="K6" s="14"/>
-      <c r="L6" s="15"/>
-      <c r="M6" s="15"/>
+      <c r="L6" s="19">
+        <v>0</v>
+      </c>
+      <c r="M6" s="19">
+        <v>5</v>
+      </c>
       <c r="N6" s="7"/>
       <c r="O6" s="7"/>
       <c r="P6" s="7"/>
@@ -834,38 +840,28 @@
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="13" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>26</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
-      <c r="F7" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="G7" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="H7" s="15" t="s">
-        <v>28</v>
-      </c>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
       <c r="I7" s="14"/>
       <c r="J7" s="15"/>
       <c r="K7" s="14"/>
-      <c r="L7" s="15">
-        <v>0</v>
-      </c>
-      <c r="M7" s="15">
-        <v>6.8579999999999997</v>
-      </c>
+      <c r="L7" s="17"/>
+      <c r="M7" s="17"/>
       <c r="N7" s="7"/>
       <c r="O7" s="7"/>
       <c r="P7" s="7"/>
@@ -882,10 +878,10 @@
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="13" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C8" s="13" t="s">
         <v>15</v>
@@ -900,19 +896,19 @@
         <v>15</v>
       </c>
       <c r="G8" s="15" t="s">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="H8" s="15" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I8" s="14"/>
       <c r="J8" s="15"/>
       <c r="K8" s="14"/>
-      <c r="L8" s="15">
-        <v>0</v>
+      <c r="L8" s="17">
+        <v>1</v>
       </c>
-      <c r="M8" s="15">
-        <v>11.557</v>
+      <c r="M8" s="18">
+        <v>1</v>
       </c>
       <c r="N8" s="7"/>
       <c r="O8" s="7"/>
@@ -930,38 +926,28 @@
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>26</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
-      <c r="F9" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="G9" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="H9" s="15" t="s">
-        <v>28</v>
-      </c>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
       <c r="I9" s="14"/>
       <c r="J9" s="15"/>
       <c r="K9" s="14"/>
-      <c r="L9" s="17">
-        <v>0</v>
-      </c>
-      <c r="M9" s="18">
-        <v>5</v>
-      </c>
+      <c r="L9" s="15"/>
+      <c r="M9" s="15"/>
       <c r="N9" s="7"/>
       <c r="O9" s="7"/>
       <c r="P9" s="7"/>
@@ -978,10 +964,10 @@
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="13" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="C10" s="13" t="s">
         <v>15</v>
@@ -996,19 +982,19 @@
         <v>15</v>
       </c>
       <c r="G10" s="15" t="s">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="H10" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I10" s="14"/>
       <c r="J10" s="15"/>
       <c r="K10" s="14"/>
-      <c r="L10" s="19">
+      <c r="L10" s="15">
         <v>0</v>
       </c>
-      <c r="M10" s="19">
-        <v>5</v>
+      <c r="M10" s="15">
+        <v>6.8579999999999997</v>
       </c>
       <c r="N10" s="7"/>
       <c r="O10" s="7"/>
@@ -1026,28 +1012,38 @@
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="13" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>26</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="15"/>
+      <c r="F11" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="H11" s="15" t="s">
+        <v>28</v>
+      </c>
       <c r="I11" s="14"/>
       <c r="J11" s="15"/>
       <c r="K11" s="14"/>
-      <c r="L11" s="17"/>
-      <c r="M11" s="18"/>
+      <c r="L11" s="15">
+        <v>0</v>
+      </c>
+      <c r="M11" s="15">
+        <v>11.557</v>
+      </c>
       <c r="N11" s="7"/>
       <c r="O11" s="7"/>
       <c r="P11" s="7"/>
@@ -1064,7 +1060,7 @@
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="13" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B12" s="13" t="s">
         <v>60</v>
@@ -1082,19 +1078,19 @@
         <v>15</v>
       </c>
       <c r="G12" s="15" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="H12" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I12" s="14"/>
       <c r="J12" s="15"/>
       <c r="K12" s="14"/>
-      <c r="L12" s="17">
+      <c r="L12" s="15">
         <v>0</v>
       </c>
-      <c r="M12" s="18">
-        <v>1</v>
+      <c r="M12" s="15">
+        <v>1.27</v>
       </c>
       <c r="N12" s="7"/>
       <c r="O12" s="7"/>
@@ -1112,28 +1108,38 @@
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="13" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D13" s="14" t="s">
         <v>26</v>
       </c>
       <c r="E13" s="13" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
-      <c r="F13" s="15"/>
-      <c r="G13" s="15"/>
-      <c r="H13" s="15"/>
+      <c r="F13" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="G13" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="H13" s="15" t="s">
+        <v>28</v>
+      </c>
       <c r="I13" s="14"/>
       <c r="J13" s="15"/>
       <c r="K13" s="14"/>
-      <c r="L13" s="17"/>
-      <c r="M13" s="17"/>
+      <c r="L13" s="15">
+        <v>0</v>
+      </c>
+      <c r="M13" s="15">
+        <v>1.4224000000000001</v>
+      </c>
       <c r="N13" s="7"/>
       <c r="O13" s="7"/>
       <c r="P13" s="7"/>
@@ -1150,28 +1156,38 @@
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="B14" s="20" t="s">
         <v>57</v>
       </c>
+      <c r="B14" s="13" t="s">
+        <v>62</v>
+      </c>
       <c r="C14" s="13" t="s">
-        <v>46</v>
+        <v>15</v>
       </c>
       <c r="D14" s="14" t="s">
         <v>26</v>
       </c>
       <c r="E14" s="13" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
-      <c r="F14" s="15"/>
-      <c r="G14" s="15"/>
-      <c r="H14" s="15"/>
+      <c r="F14" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="G14" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="H14" s="15" t="s">
+        <v>28</v>
+      </c>
       <c r="I14" s="14"/>
       <c r="J14" s="15"/>
       <c r="K14" s="14"/>
-      <c r="L14" s="15"/>
-      <c r="M14" s="15"/>
+      <c r="L14" s="15">
+        <v>0</v>
+      </c>
+      <c r="M14" s="15">
+        <v>0.93979999999999997</v>
+      </c>
       <c r="N14" s="7"/>
       <c r="O14" s="7"/>
       <c r="P14" s="7"/>
@@ -1188,13 +1204,13 @@
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="13" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="B15" s="20" t="s">
         <v>58</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>26</v>
@@ -1208,8 +1224,8 @@
       <c r="I15" s="14"/>
       <c r="J15" s="15"/>
       <c r="K15" s="14"/>
-      <c r="L15" s="16"/>
-      <c r="M15" s="16"/>
+      <c r="L15" s="15"/>
+      <c r="M15" s="15"/>
       <c r="N15" s="7"/>
       <c r="O15" s="7"/>
       <c r="P15" s="7"/>
@@ -1226,13 +1242,13 @@
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="13" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="B16" s="20" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="D16" s="14" t="s">
         <v>26</v>
@@ -1246,8 +1262,8 @@
       <c r="I16" s="14"/>
       <c r="J16" s="15"/>
       <c r="K16" s="14"/>
-      <c r="L16" s="21"/>
-      <c r="M16" s="15"/>
+      <c r="L16" s="16"/>
+      <c r="M16" s="16"/>
       <c r="N16" s="7"/>
       <c r="O16" s="7"/>
       <c r="P16" s="7"/>
@@ -1263,19 +1279,29 @@
       <c r="Z16" s="7"/>
     </row>
     <row r="17" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="6"/>
-      <c r="K17" s="5"/>
-      <c r="L17" s="9"/>
-      <c r="M17" s="6"/>
+      <c r="A17" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E17" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="15"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="15"/>
+      <c r="K17" s="14"/>
+      <c r="L17" s="21"/>
+      <c r="M17" s="15"/>
       <c r="N17" s="7"/>
       <c r="O17" s="7"/>
       <c r="P17" s="7"/>
@@ -1291,19 +1317,39 @@
       <c r="Z17" s="7"/>
     </row>
     <row r="18" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="6"/>
-      <c r="K18" s="5"/>
-      <c r="L18" s="9"/>
-      <c r="M18" s="6"/>
+      <c r="A18" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E18" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F18" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="G18" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="H18" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="I18" s="14"/>
+      <c r="J18" s="15"/>
+      <c r="K18" s="14"/>
+      <c r="L18" s="17">
+        <v>0</v>
+      </c>
+      <c r="M18" s="18">
+        <v>5</v>
+      </c>
       <c r="N18" s="7"/>
       <c r="O18" s="7"/>
       <c r="P18" s="7"/>
@@ -1330,8 +1376,8 @@
       <c r="I19" s="5"/>
       <c r="J19" s="6"/>
       <c r="K19" s="5"/>
-      <c r="L19" s="10"/>
-      <c r="M19" s="10"/>
+      <c r="L19" s="9"/>
+      <c r="M19" s="6"/>
       <c r="N19" s="7"/>
       <c r="O19" s="7"/>
       <c r="P19" s="7"/>
@@ -1359,7 +1405,7 @@
       <c r="J20" s="6"/>
       <c r="K20" s="5"/>
       <c r="L20" s="10"/>
-      <c r="M20" s="6"/>
+      <c r="M20" s="10"/>
       <c r="N20" s="7"/>
       <c r="O20" s="7"/>
       <c r="P20" s="7"/>
@@ -1414,7 +1460,7 @@
       <c r="I22" s="5"/>
       <c r="J22" s="6"/>
       <c r="K22" s="5"/>
-      <c r="L22" s="9"/>
+      <c r="L22" s="10"/>
       <c r="M22" s="6"/>
       <c r="N22" s="7"/>
       <c r="O22" s="7"/>
@@ -1432,18 +1478,18 @@
     </row>
     <row r="23" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="4"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="11"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="12"/>
-      <c r="G23" s="12"/>
-      <c r="H23" s="12"/>
-      <c r="I23" s="11"/>
-      <c r="J23" s="12"/>
-      <c r="K23" s="11"/>
-      <c r="L23" s="12"/>
-      <c r="M23" s="12"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="5"/>
+      <c r="J23" s="6"/>
+      <c r="K23" s="5"/>
+      <c r="L23" s="9"/>
+      <c r="M23" s="6"/>
       <c r="N23" s="7"/>
       <c r="O23" s="7"/>
       <c r="P23" s="7"/>
@@ -1542,8 +1588,9 @@
       <c r="Y26" s="7"/>
       <c r="Z26" s="7"/>
     </row>
-    <row r="27" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="4"/>
+      <c r="B27" s="7"/>
       <c r="C27" s="7"/>
       <c r="D27" s="11"/>
       <c r="E27" s="7"/>
@@ -1569,9 +1616,8 @@
       <c r="Y27" s="7"/>
       <c r="Z27" s="7"/>
     </row>
-    <row r="28" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="4"/>
-      <c r="B28" s="7"/>
       <c r="C28" s="7"/>
       <c r="D28" s="11"/>
       <c r="E28" s="7"/>
@@ -1739,34 +1785,34 @@
     </row>
     <row r="34" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="4"/>
+      <c r="B34" s="7"/>
       <c r="C34" s="7"/>
       <c r="D34" s="11"/>
       <c r="E34" s="7"/>
-      <c r="F34" s="6"/>
-      <c r="G34" s="6"/>
-      <c r="H34" s="6"/>
-      <c r="I34" s="5"/>
-      <c r="J34" s="6"/>
-      <c r="K34" s="5"/>
-      <c r="L34" s="6"/>
-      <c r="M34" s="6"/>
-      <c r="N34" s="4"/>
-      <c r="O34" s="4"/>
-      <c r="P34" s="4"/>
-      <c r="Q34" s="4"/>
-      <c r="R34" s="4"/>
-      <c r="S34" s="4"/>
-      <c r="T34" s="4"/>
-      <c r="U34" s="4"/>
-      <c r="V34" s="4"/>
-      <c r="W34" s="4"/>
-      <c r="X34" s="4"/>
-      <c r="Y34" s="4"/>
-      <c r="Z34" s="4"/>
+      <c r="F34" s="12"/>
+      <c r="G34" s="12"/>
+      <c r="H34" s="12"/>
+      <c r="I34" s="11"/>
+      <c r="J34" s="12"/>
+      <c r="K34" s="11"/>
+      <c r="L34" s="12"/>
+      <c r="M34" s="12"/>
+      <c r="N34" s="7"/>
+      <c r="O34" s="7"/>
+      <c r="P34" s="7"/>
+      <c r="Q34" s="7"/>
+      <c r="R34" s="7"/>
+      <c r="S34" s="7"/>
+      <c r="T34" s="7"/>
+      <c r="U34" s="7"/>
+      <c r="V34" s="7"/>
+      <c r="W34" s="7"/>
+      <c r="X34" s="7"/>
+      <c r="Y34" s="7"/>
+      <c r="Z34" s="7"/>
     </row>
     <row r="35" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="4"/>
-      <c r="B35" s="7"/>
       <c r="C35" s="7"/>
       <c r="D35" s="11"/>
       <c r="E35" s="7"/>
@@ -1798,29 +1844,39 @@
       <c r="C36" s="7"/>
       <c r="D36" s="11"/>
       <c r="E36" s="7"/>
-      <c r="F36" s="12"/>
-      <c r="G36" s="12"/>
-      <c r="H36" s="12"/>
-      <c r="I36" s="11"/>
-      <c r="J36" s="12"/>
-      <c r="K36" s="11"/>
-      <c r="L36" s="12"/>
-      <c r="M36" s="12"/>
-      <c r="N36" s="7"/>
-      <c r="O36" s="7"/>
-      <c r="P36" s="7"/>
-      <c r="Q36" s="7"/>
-      <c r="R36" s="7"/>
-      <c r="S36" s="7"/>
-      <c r="T36" s="7"/>
-      <c r="U36" s="7"/>
-      <c r="V36" s="7"/>
-      <c r="W36" s="7"/>
-      <c r="X36" s="7"/>
-      <c r="Y36" s="7"/>
-      <c r="Z36" s="7"/>
+      <c r="F36" s="6"/>
+      <c r="G36" s="6"/>
+      <c r="H36" s="6"/>
+      <c r="I36" s="5"/>
+      <c r="J36" s="6"/>
+      <c r="K36" s="5"/>
+      <c r="L36" s="6"/>
+      <c r="M36" s="6"/>
+      <c r="N36" s="4"/>
+      <c r="O36" s="4"/>
+      <c r="P36" s="4"/>
+      <c r="Q36" s="4"/>
+      <c r="R36" s="4"/>
+      <c r="S36" s="4"/>
+      <c r="T36" s="4"/>
+      <c r="U36" s="4"/>
+      <c r="V36" s="4"/>
+      <c r="W36" s="4"/>
+      <c r="X36" s="4"/>
+      <c r="Y36" s="4"/>
+      <c r="Z36" s="4"/>
     </row>
     <row r="37" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="4"/>
+      <c r="B37" s="7"/>
+      <c r="C37" s="7"/>
+      <c r="D37" s="11"/>
+      <c r="E37" s="7"/>
+      <c r="F37" s="12"/>
+      <c r="G37" s="12"/>
+      <c r="H37" s="12"/>
+      <c r="I37" s="11"/>
+      <c r="J37" s="12"/>
       <c r="K37" s="11"/>
       <c r="L37" s="12"/>
       <c r="M37" s="12"/>
@@ -1839,16 +1895,6 @@
       <c r="Z37" s="7"/>
     </row>
     <row r="38" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="4"/>
-      <c r="B38" s="7"/>
-      <c r="C38" s="7"/>
-      <c r="D38" s="11"/>
-      <c r="E38" s="7"/>
-      <c r="F38" s="12"/>
-      <c r="G38" s="12"/>
-      <c r="H38" s="12"/>
-      <c r="I38" s="11"/>
-      <c r="J38" s="12"/>
       <c r="K38" s="11"/>
       <c r="L38" s="12"/>
       <c r="M38" s="12"/>
@@ -1979,6 +2025,7 @@
       <c r="Z42" s="7"/>
     </row>
     <row r="43" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="4"/>
       <c r="B43" s="7"/>
       <c r="C43" s="7"/>
       <c r="D43" s="11"/>
@@ -2006,7 +2053,6 @@
       <c r="Z43" s="7"/>
     </row>
     <row r="44" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="4"/>
       <c r="B44" s="7"/>
       <c r="C44" s="7"/>
       <c r="D44" s="11"/>
@@ -2034,6 +2080,7 @@
       <c r="Z44" s="7"/>
     </row>
     <row r="45" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="4"/>
       <c r="B45" s="7"/>
       <c r="C45" s="7"/>
       <c r="D45" s="11"/>
@@ -2061,7 +2108,6 @@
       <c r="Z45" s="7"/>
     </row>
     <row r="46" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="4"/>
       <c r="B46" s="7"/>
       <c r="C46" s="7"/>
       <c r="D46" s="11"/>
@@ -3013,7 +3059,7 @@
       <c r="Z79" s="7"/>
     </row>
     <row r="80" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="7"/>
+      <c r="A80" s="4"/>
       <c r="B80" s="7"/>
       <c r="C80" s="7"/>
       <c r="D80" s="11"/>
@@ -28940,18 +28986,46 @@
       <c r="Y1005" s="7"/>
       <c r="Z1005" s="7"/>
     </row>
+    <row r="1006" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1006" s="7"/>
+      <c r="B1006" s="7"/>
+      <c r="C1006" s="7"/>
+      <c r="D1006" s="11"/>
+      <c r="E1006" s="7"/>
+      <c r="F1006" s="12"/>
+      <c r="G1006" s="12"/>
+      <c r="H1006" s="12"/>
+      <c r="I1006" s="11"/>
+      <c r="J1006" s="12"/>
+      <c r="K1006" s="11"/>
+      <c r="L1006" s="12"/>
+      <c r="M1006" s="12"/>
+      <c r="N1006" s="7"/>
+      <c r="O1006" s="7"/>
+      <c r="P1006" s="7"/>
+      <c r="Q1006" s="7"/>
+      <c r="R1006" s="7"/>
+      <c r="S1006" s="7"/>
+      <c r="T1006" s="7"/>
+      <c r="U1006" s="7"/>
+      <c r="V1006" s="7"/>
+      <c r="W1006" s="7"/>
+      <c r="X1006" s="7"/>
+      <c r="Y1006" s="7"/>
+      <c r="Z1006" s="7"/>
+    </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C62:C1005 C38:C50 C1:C36" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C63:C1006 C39:C51 C15:C37 C1:C14" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"nominal,ordinal,interval,ratio,dateTime"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E38:E1005 E1:E36" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E39:E1006 E15:E37 E1:E14" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"text,enumerated,dateTime,numeric"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F38:F1005 F1:F36" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F39:F1006 F15:F37 F1:F14" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"ratio,interval"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H38:H1005 H1:H36" xr:uid="{00000000-0002-0000-0000-000003000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H39:H1006 H15:H37 H1:H14" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"natural,whole,integer,real"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
updates make_metadata_xml to reflect new naming conventions for escapement, validates .xml, and debugs metadata
</commit_message>
<xml_diff>
--- a/data-raw/metadata/battle_redd_metadata.xlsx
+++ b/data-raw/metadata/battle_redd_metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/code/SRJPE/EDI/jpe-battle-adult-edi/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27B69B56-A4BF-8843-9EDB-7205F30DFB3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EFEBF9D-CCDE-4B49-B149-8D630AB91F97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="68640" yWindow="-9480" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="66">
   <si>
     <t xml:space="preserve">attribute_name </t>
   </si>
@@ -563,7 +563,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="147" zoomScaleNormal="147" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
+      <selection pane="bottomLeft" activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -689,9 +689,15 @@
       <c r="B3" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="C3" s="13"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="13"/>
+      <c r="C3" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>14</v>
+      </c>
       <c r="F3" s="15"/>
       <c r="G3" s="15"/>
       <c r="H3" s="15"/>
@@ -29016,16 +29022,16 @@
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C63:C1006 C39:C51 C15:C37 C1:C14" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C63:C1006 C39:C51 C1:C37" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"nominal,ordinal,interval,ratio,dateTime"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E39:E1006 E15:E37 E1:E14" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E39:E1006 E1:E37" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"text,enumerated,dateTime,numeric"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F39:F1006 F15:F37 F1:F14" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F39:F1006 F1:F37" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"ratio,interval"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H39:H1006 H15:H37 H1:H14" xr:uid="{00000000-0002-0000-0000-000003000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H39:H1006 H1:H37" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"natural,whole,integer,real"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
updates metadata and xml
</commit_message>
<xml_diff>
--- a/data-raw/metadata/battle_redd_metadata.xlsx
+++ b/data-raw/metadata/battle_redd_metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/code/SRJPE/EDI/jpe-battle-adult-edi/data-raw/metadata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashleyvizek/code/jpe-battle-adult-edi/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EFEBF9D-CCDE-4B49-B149-8D630AB91F97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E3866DE-12FA-B146-8DBF-B420D6BD3C06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="68640" yWindow="-9480" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="63">
   <si>
     <t xml:space="preserve">attribute_name </t>
   </si>
@@ -169,12 +169,6 @@
     <t>year</t>
   </si>
   <si>
-    <t>redd_count</t>
-  </si>
-  <si>
-    <t>number of redds</t>
-  </si>
-  <si>
     <t>redd_id</t>
   </si>
   <si>
@@ -188,9 +182,6 @@
   </si>
   <si>
     <t>Run of the fish on the redd. Levels = c("spring", NA)</t>
-  </si>
-  <si>
-    <t>Number of redds sampled.</t>
   </si>
   <si>
     <t>pre_redd_depth</t>
@@ -559,11 +550,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1006"/>
+  <dimension ref="A1:Z1005"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="147" zoomScaleNormal="147" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H4" sqref="H4"/>
+      <selection pane="bottomLeft" activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -643,7 +634,7 @@
         <v>21</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C2" s="13" t="s">
         <v>17</v>
@@ -684,10 +675,10 @@
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C3" s="13" t="s">
         <v>38</v>
@@ -725,7 +716,7 @@
         <v>32</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C4" s="13" t="s">
         <v>13</v>
@@ -760,10 +751,10 @@
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C5" s="13" t="s">
         <v>13</v>
@@ -849,7 +840,7 @@
         <v>37</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C7" s="13" t="s">
         <v>13</v>
@@ -884,38 +875,28 @@
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="13" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D8" s="14" t="s">
         <v>26</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
-      <c r="F8" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="G8" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="H8" s="15" t="s">
-        <v>29</v>
-      </c>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
       <c r="I8" s="14"/>
       <c r="J8" s="15"/>
       <c r="K8" s="14"/>
-      <c r="L8" s="17">
-        <v>1</v>
-      </c>
-      <c r="M8" s="18">
-        <v>1</v>
-      </c>
+      <c r="L8" s="15"/>
+      <c r="M8" s="15"/>
       <c r="N8" s="7"/>
       <c r="O8" s="7"/>
       <c r="P8" s="7"/>
@@ -932,28 +913,38 @@
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>26</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="15"/>
+      <c r="F9" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="H9" s="15" t="s">
+        <v>28</v>
+      </c>
       <c r="I9" s="14"/>
       <c r="J9" s="15"/>
       <c r="K9" s="14"/>
-      <c r="L9" s="15"/>
-      <c r="M9" s="15"/>
+      <c r="L9" s="15">
+        <v>0</v>
+      </c>
+      <c r="M9" s="15">
+        <v>6.8579999999999997</v>
+      </c>
       <c r="N9" s="7"/>
       <c r="O9" s="7"/>
       <c r="P9" s="7"/>
@@ -970,10 +961,10 @@
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="13" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C10" s="13" t="s">
         <v>15</v>
@@ -1000,7 +991,7 @@
         <v>0</v>
       </c>
       <c r="M10" s="15">
-        <v>6.8579999999999997</v>
+        <v>11.557</v>
       </c>
       <c r="N10" s="7"/>
       <c r="O10" s="7"/>
@@ -1018,10 +1009,10 @@
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="13" t="s">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="C11" s="13" t="s">
         <v>15</v>
@@ -1036,7 +1027,7 @@
         <v>15</v>
       </c>
       <c r="G11" s="15" t="s">
-        <v>25</v>
+        <v>60</v>
       </c>
       <c r="H11" s="15" t="s">
         <v>28</v>
@@ -1048,7 +1039,7 @@
         <v>0</v>
       </c>
       <c r="M11" s="15">
-        <v>11.557</v>
+        <v>1.27</v>
       </c>
       <c r="N11" s="7"/>
       <c r="O11" s="7"/>
@@ -1066,10 +1057,10 @@
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="13" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C12" s="13" t="s">
         <v>15</v>
@@ -1084,7 +1075,7 @@
         <v>15</v>
       </c>
       <c r="G12" s="15" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="H12" s="15" t="s">
         <v>28</v>
@@ -1096,7 +1087,7 @@
         <v>0</v>
       </c>
       <c r="M12" s="15">
-        <v>1.27</v>
+        <v>1.4224000000000001</v>
       </c>
       <c r="N12" s="7"/>
       <c r="O12" s="7"/>
@@ -1114,10 +1105,10 @@
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="13" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C13" s="13" t="s">
         <v>15</v>
@@ -1132,7 +1123,7 @@
         <v>15</v>
       </c>
       <c r="G13" s="15" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="H13" s="15" t="s">
         <v>28</v>
@@ -1144,7 +1135,7 @@
         <v>0</v>
       </c>
       <c r="M13" s="15">
-        <v>1.4224000000000001</v>
+        <v>0.93979999999999997</v>
       </c>
       <c r="N13" s="7"/>
       <c r="O13" s="7"/>
@@ -1162,38 +1153,28 @@
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="13" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
-      <c r="B14" s="13" t="s">
-        <v>62</v>
+      <c r="B14" s="20" t="s">
+        <v>55</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="D14" s="14" t="s">
         <v>26</v>
       </c>
       <c r="E14" s="13" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
-      <c r="F14" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="G14" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="H14" s="15" t="s">
-        <v>28</v>
-      </c>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
       <c r="I14" s="14"/>
       <c r="J14" s="15"/>
       <c r="K14" s="14"/>
-      <c r="L14" s="15">
-        <v>0</v>
-      </c>
-      <c r="M14" s="15">
-        <v>0.93979999999999997</v>
-      </c>
+      <c r="L14" s="15"/>
+      <c r="M14" s="15"/>
       <c r="N14" s="7"/>
       <c r="O14" s="7"/>
       <c r="P14" s="7"/>
@@ -1210,10 +1191,10 @@
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="13" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B15" s="20" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C15" s="13" t="s">
         <v>38</v>
@@ -1230,8 +1211,8 @@
       <c r="I15" s="14"/>
       <c r="J15" s="15"/>
       <c r="K15" s="14"/>
-      <c r="L15" s="15"/>
-      <c r="M15" s="15"/>
+      <c r="L15" s="16"/>
+      <c r="M15" s="16"/>
       <c r="N15" s="7"/>
       <c r="O15" s="7"/>
       <c r="P15" s="7"/>
@@ -1248,10 +1229,10 @@
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="13" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B16" s="20" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C16" s="13" t="s">
         <v>38</v>
@@ -1268,8 +1249,8 @@
       <c r="I16" s="14"/>
       <c r="J16" s="15"/>
       <c r="K16" s="14"/>
-      <c r="L16" s="16"/>
-      <c r="M16" s="16"/>
+      <c r="L16" s="21"/>
+      <c r="M16" s="15"/>
       <c r="N16" s="7"/>
       <c r="O16" s="7"/>
       <c r="P16" s="7"/>
@@ -1286,28 +1267,38 @@
     </row>
     <row r="17" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="13" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
-      <c r="B17" s="20" t="s">
-        <v>58</v>
+      <c r="B17" s="13" t="s">
+        <v>23</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>38</v>
+        <v>15</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>26</v>
       </c>
       <c r="E17" s="13" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
-      <c r="F17" s="15"/>
-      <c r="G17" s="15"/>
-      <c r="H17" s="15"/>
+      <c r="F17" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="G17" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="H17" s="15" t="s">
+        <v>28</v>
+      </c>
       <c r="I17" s="14"/>
       <c r="J17" s="15"/>
       <c r="K17" s="14"/>
-      <c r="L17" s="21"/>
-      <c r="M17" s="15"/>
+      <c r="L17" s="17">
+        <v>0</v>
+      </c>
+      <c r="M17" s="18">
+        <v>5</v>
+      </c>
       <c r="N17" s="7"/>
       <c r="O17" s="7"/>
       <c r="P17" s="7"/>
@@ -1323,39 +1314,19 @@
       <c r="Z17" s="7"/>
     </row>
     <row r="18" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="B18" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="C18" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="D18" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="E18" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="F18" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="G18" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="H18" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="I18" s="14"/>
-      <c r="J18" s="15"/>
-      <c r="K18" s="14"/>
-      <c r="L18" s="17">
-        <v>0</v>
-      </c>
-      <c r="M18" s="18">
-        <v>5</v>
-      </c>
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="5"/>
+      <c r="L18" s="9"/>
+      <c r="M18" s="6"/>
       <c r="N18" s="7"/>
       <c r="O18" s="7"/>
       <c r="P18" s="7"/>
@@ -1382,8 +1353,8 @@
       <c r="I19" s="5"/>
       <c r="J19" s="6"/>
       <c r="K19" s="5"/>
-      <c r="L19" s="9"/>
-      <c r="M19" s="6"/>
+      <c r="L19" s="10"/>
+      <c r="M19" s="10"/>
       <c r="N19" s="7"/>
       <c r="O19" s="7"/>
       <c r="P19" s="7"/>
@@ -1411,7 +1382,7 @@
       <c r="J20" s="6"/>
       <c r="K20" s="5"/>
       <c r="L20" s="10"/>
-      <c r="M20" s="10"/>
+      <c r="M20" s="6"/>
       <c r="N20" s="7"/>
       <c r="O20" s="7"/>
       <c r="P20" s="7"/>
@@ -1466,7 +1437,7 @@
       <c r="I22" s="5"/>
       <c r="J22" s="6"/>
       <c r="K22" s="5"/>
-      <c r="L22" s="10"/>
+      <c r="L22" s="9"/>
       <c r="M22" s="6"/>
       <c r="N22" s="7"/>
       <c r="O22" s="7"/>
@@ -1484,18 +1455,18 @@
     </row>
     <row r="23" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="4"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="5"/>
-      <c r="J23" s="6"/>
-      <c r="K23" s="5"/>
-      <c r="L23" s="9"/>
-      <c r="M23" s="6"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="12"/>
+      <c r="I23" s="11"/>
+      <c r="J23" s="12"/>
+      <c r="K23" s="11"/>
+      <c r="L23" s="12"/>
+      <c r="M23" s="12"/>
       <c r="N23" s="7"/>
       <c r="O23" s="7"/>
       <c r="P23" s="7"/>
@@ -1594,9 +1565,8 @@
       <c r="Y26" s="7"/>
       <c r="Z26" s="7"/>
     </row>
-    <row r="27" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="4"/>
-      <c r="B27" s="7"/>
       <c r="C27" s="7"/>
       <c r="D27" s="11"/>
       <c r="E27" s="7"/>
@@ -1622,8 +1592,9 @@
       <c r="Y27" s="7"/>
       <c r="Z27" s="7"/>
     </row>
-    <row r="28" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="4"/>
+      <c r="B28" s="7"/>
       <c r="C28" s="7"/>
       <c r="D28" s="11"/>
       <c r="E28" s="7"/>
@@ -1791,34 +1762,34 @@
     </row>
     <row r="34" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="4"/>
-      <c r="B34" s="7"/>
       <c r="C34" s="7"/>
       <c r="D34" s="11"/>
       <c r="E34" s="7"/>
-      <c r="F34" s="12"/>
-      <c r="G34" s="12"/>
-      <c r="H34" s="12"/>
-      <c r="I34" s="11"/>
-      <c r="J34" s="12"/>
-      <c r="K34" s="11"/>
-      <c r="L34" s="12"/>
-      <c r="M34" s="12"/>
-      <c r="N34" s="7"/>
-      <c r="O34" s="7"/>
-      <c r="P34" s="7"/>
-      <c r="Q34" s="7"/>
-      <c r="R34" s="7"/>
-      <c r="S34" s="7"/>
-      <c r="T34" s="7"/>
-      <c r="U34" s="7"/>
-      <c r="V34" s="7"/>
-      <c r="W34" s="7"/>
-      <c r="X34" s="7"/>
-      <c r="Y34" s="7"/>
-      <c r="Z34" s="7"/>
+      <c r="F34" s="6"/>
+      <c r="G34" s="6"/>
+      <c r="H34" s="6"/>
+      <c r="I34" s="5"/>
+      <c r="J34" s="6"/>
+      <c r="K34" s="5"/>
+      <c r="L34" s="6"/>
+      <c r="M34" s="6"/>
+      <c r="N34" s="4"/>
+      <c r="O34" s="4"/>
+      <c r="P34" s="4"/>
+      <c r="Q34" s="4"/>
+      <c r="R34" s="4"/>
+      <c r="S34" s="4"/>
+      <c r="T34" s="4"/>
+      <c r="U34" s="4"/>
+      <c r="V34" s="4"/>
+      <c r="W34" s="4"/>
+      <c r="X34" s="4"/>
+      <c r="Y34" s="4"/>
+      <c r="Z34" s="4"/>
     </row>
     <row r="35" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="4"/>
+      <c r="B35" s="7"/>
       <c r="C35" s="7"/>
       <c r="D35" s="11"/>
       <c r="E35" s="7"/>
@@ -1850,39 +1821,29 @@
       <c r="C36" s="7"/>
       <c r="D36" s="11"/>
       <c r="E36" s="7"/>
-      <c r="F36" s="6"/>
-      <c r="G36" s="6"/>
-      <c r="H36" s="6"/>
-      <c r="I36" s="5"/>
-      <c r="J36" s="6"/>
-      <c r="K36" s="5"/>
-      <c r="L36" s="6"/>
-      <c r="M36" s="6"/>
-      <c r="N36" s="4"/>
-      <c r="O36" s="4"/>
-      <c r="P36" s="4"/>
-      <c r="Q36" s="4"/>
-      <c r="R36" s="4"/>
-      <c r="S36" s="4"/>
-      <c r="T36" s="4"/>
-      <c r="U36" s="4"/>
-      <c r="V36" s="4"/>
-      <c r="W36" s="4"/>
-      <c r="X36" s="4"/>
-      <c r="Y36" s="4"/>
-      <c r="Z36" s="4"/>
+      <c r="F36" s="12"/>
+      <c r="G36" s="12"/>
+      <c r="H36" s="12"/>
+      <c r="I36" s="11"/>
+      <c r="J36" s="12"/>
+      <c r="K36" s="11"/>
+      <c r="L36" s="12"/>
+      <c r="M36" s="12"/>
+      <c r="N36" s="7"/>
+      <c r="O36" s="7"/>
+      <c r="P36" s="7"/>
+      <c r="Q36" s="7"/>
+      <c r="R36" s="7"/>
+      <c r="S36" s="7"/>
+      <c r="T36" s="7"/>
+      <c r="U36" s="7"/>
+      <c r="V36" s="7"/>
+      <c r="W36" s="7"/>
+      <c r="X36" s="7"/>
+      <c r="Y36" s="7"/>
+      <c r="Z36" s="7"/>
     </row>
     <row r="37" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="4"/>
-      <c r="B37" s="7"/>
-      <c r="C37" s="7"/>
-      <c r="D37" s="11"/>
-      <c r="E37" s="7"/>
-      <c r="F37" s="12"/>
-      <c r="G37" s="12"/>
-      <c r="H37" s="12"/>
-      <c r="I37" s="11"/>
-      <c r="J37" s="12"/>
       <c r="K37" s="11"/>
       <c r="L37" s="12"/>
       <c r="M37" s="12"/>
@@ -1901,6 +1862,16 @@
       <c r="Z37" s="7"/>
     </row>
     <row r="38" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="4"/>
+      <c r="B38" s="7"/>
+      <c r="C38" s="7"/>
+      <c r="D38" s="11"/>
+      <c r="E38" s="7"/>
+      <c r="F38" s="12"/>
+      <c r="G38" s="12"/>
+      <c r="H38" s="12"/>
+      <c r="I38" s="11"/>
+      <c r="J38" s="12"/>
       <c r="K38" s="11"/>
       <c r="L38" s="12"/>
       <c r="M38" s="12"/>
@@ -2031,7 +2002,6 @@
       <c r="Z42" s="7"/>
     </row>
     <row r="43" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="4"/>
       <c r="B43" s="7"/>
       <c r="C43" s="7"/>
       <c r="D43" s="11"/>
@@ -2059,6 +2029,7 @@
       <c r="Z43" s="7"/>
     </row>
     <row r="44" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="4"/>
       <c r="B44" s="7"/>
       <c r="C44" s="7"/>
       <c r="D44" s="11"/>
@@ -2086,7 +2057,6 @@
       <c r="Z44" s="7"/>
     </row>
     <row r="45" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="4"/>
       <c r="B45" s="7"/>
       <c r="C45" s="7"/>
       <c r="D45" s="11"/>
@@ -2114,6 +2084,7 @@
       <c r="Z45" s="7"/>
     </row>
     <row r="46" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="4"/>
       <c r="B46" s="7"/>
       <c r="C46" s="7"/>
       <c r="D46" s="11"/>
@@ -3065,7 +3036,7 @@
       <c r="Z79" s="7"/>
     </row>
     <row r="80" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="4"/>
+      <c r="A80" s="7"/>
       <c r="B80" s="7"/>
       <c r="C80" s="7"/>
       <c r="D80" s="11"/>
@@ -28992,46 +28963,18 @@
       <c r="Y1005" s="7"/>
       <c r="Z1005" s="7"/>
     </row>
-    <row r="1006" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1006" s="7"/>
-      <c r="B1006" s="7"/>
-      <c r="C1006" s="7"/>
-      <c r="D1006" s="11"/>
-      <c r="E1006" s="7"/>
-      <c r="F1006" s="12"/>
-      <c r="G1006" s="12"/>
-      <c r="H1006" s="12"/>
-      <c r="I1006" s="11"/>
-      <c r="J1006" s="12"/>
-      <c r="K1006" s="11"/>
-      <c r="L1006" s="12"/>
-      <c r="M1006" s="12"/>
-      <c r="N1006" s="7"/>
-      <c r="O1006" s="7"/>
-      <c r="P1006" s="7"/>
-      <c r="Q1006" s="7"/>
-      <c r="R1006" s="7"/>
-      <c r="S1006" s="7"/>
-      <c r="T1006" s="7"/>
-      <c r="U1006" s="7"/>
-      <c r="V1006" s="7"/>
-      <c r="W1006" s="7"/>
-      <c r="X1006" s="7"/>
-      <c r="Y1006" s="7"/>
-      <c r="Z1006" s="7"/>
-    </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C63:C1006 C39:C51 C1:C37" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C62:C1005 C38:C50 C1:C36" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"nominal,ordinal,interval,ratio,dateTime"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E39:E1006 E1:E37" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E38:E1005 E1:E36" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"text,enumerated,dateTime,numeric"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F39:F1006 F1:F37" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F38:F1005 F1:F36" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"ratio,interval"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H39:H1006 H1:H37" xr:uid="{00000000-0002-0000-0000-000003000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H38:H1005 H1:H36" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"natural,whole,integer,real"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>